<commit_message>
add the sir_model function, needs debugging
</commit_message>
<xml_diff>
--- a/graph_info.xlsx
+++ b/graph_info.xlsx
@@ -506,13 +506,13 @@
         <v>9.949999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04154400974694425</v>
+        <v>0.04575443874290686</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
@@ -543,13 +543,13 @@
         <v>19.8</v>
       </c>
       <c r="E3" t="n">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="F3" t="n">
         <v>10</v>
       </c>
       <c r="G3" t="n">
-        <v>0.06076746020758292</v>
+        <v>0.06324657660138239</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -580,13 +580,13 @@
         <v>3.992</v>
       </c>
       <c r="E4" t="n">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0189560524449966</v>
+        <v>0.02267945347652807</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -617,13 +617,13 @@
         <v>9.975</v>
       </c>
       <c r="E5" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F5" t="n">
         <v>5</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0236089709335522</v>
+        <v>0.02162823772088771</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -654,13 +654,13 @@
         <v>19.9</v>
       </c>
       <c r="E6" t="n">
-        <v>214</v>
+        <v>261</v>
       </c>
       <c r="F6" t="n">
         <v>10</v>
       </c>
       <c r="G6" t="n">
-        <v>0.03757370621423827</v>
+        <v>0.03922053475144366</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -691,13 +691,13 @@
         <v>3.996</v>
       </c>
       <c r="E7" t="n">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01207031230168897</v>
+        <v>0.01061226102384237</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
@@ -728,13 +728,13 @@
         <v>9.983333333333333</v>
       </c>
       <c r="E8" t="n">
-        <v>267</v>
+        <v>231</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01747714527877825</v>
+        <v>0.01810323634571336</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -765,13 +765,13 @@
         <v>19.93333333333333</v>
       </c>
       <c r="E9" t="n">
-        <v>291</v>
+        <v>247</v>
       </c>
       <c r="F9" t="n">
         <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>0.02823195264140716</v>
+        <v>0.02660723692926331</v>
       </c>
       <c r="H9" t="n">
         <v>1</v>
@@ -802,13 +802,13 @@
         <v>3.997333333333333</v>
       </c>
       <c r="E10" t="n">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F10" t="n">
         <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01168288714479156</v>
+        <v>0.01378842105240141</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
@@ -839,13 +839,13 @@
         <v>3.997333333333333</v>
       </c>
       <c r="E11" t="n">
-        <v>198</v>
+        <v>116</v>
       </c>
       <c r="F11" t="n">
         <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01551116481975751</v>
+        <v>0.009469554293510648</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
@@ -876,13 +876,13 @@
         <v>3.998</v>
       </c>
       <c r="E12" t="n">
-        <v>280</v>
+        <v>111</v>
       </c>
       <c r="F12" t="n">
         <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01163634515937211</v>
+        <v>0.007281291733332003</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
@@ -913,13 +913,13 @@
         <v>3.9984</v>
       </c>
       <c r="E13" t="n">
-        <v>160</v>
+        <v>277</v>
       </c>
       <c r="F13" t="n">
         <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>0.006769571735316574</v>
+        <v>0.008819291968009482</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -950,13 +950,13 @@
         <v>3.998666666666667</v>
       </c>
       <c r="E14" t="n">
-        <v>182</v>
+        <v>251</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>0.006797036761107506</v>
+        <v>0.00598171552042424</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
@@ -987,13 +987,13 @@
         <v>3.998857142857143</v>
       </c>
       <c r="E15" t="n">
-        <v>257</v>
+        <v>214</v>
       </c>
       <c r="F15" t="n">
         <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>0.006227718991588389</v>
+        <v>0.00670081302902699</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
@@ -1024,13 +1024,13 @@
         <v>3.999</v>
       </c>
       <c r="E16" t="n">
-        <v>216</v>
+        <v>326</v>
       </c>
       <c r="F16" t="n">
         <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>0.005674033442492185</v>
+        <v>0.007949204903071607</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
@@ -1061,13 +1061,13 @@
         <v>9.975</v>
       </c>
       <c r="E17" t="n">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="F17" t="n">
         <v>5</v>
       </c>
       <c r="G17" t="n">
-        <v>0.02247085556250707</v>
+        <v>0.02598671790384382</v>
       </c>
       <c r="H17" t="n">
         <v>1</v>
@@ -1098,13 +1098,13 @@
         <v>19.9</v>
       </c>
       <c r="E18" t="n">
-        <v>292</v>
+        <v>233</v>
       </c>
       <c r="F18" t="n">
         <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>0.03710269777573309</v>
+        <v>0.03692968282165096</v>
       </c>
       <c r="H18" t="n">
         <v>1</v>
@@ -1135,13 +1135,13 @@
         <v>3.996</v>
       </c>
       <c r="E19" t="n">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>0.01097441645643306</v>
+        <v>0.01366432290567512</v>
       </c>
       <c r="H19" t="n">
         <v>1</v>
@@ -1172,13 +1172,13 @@
         <v>9.987500000000001</v>
       </c>
       <c r="E20" t="n">
-        <v>278</v>
+        <v>188</v>
       </c>
       <c r="F20" t="n">
         <v>5</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01455914259780427</v>
+        <v>0.01301287560234095</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
@@ -1209,7 +1209,7 @@
         <v>1.9995</v>
       </c>
       <c r="E21" t="n">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
@@ -1246,13 +1246,13 @@
         <v>5.9955</v>
       </c>
       <c r="E22" t="n">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F22" t="n">
         <v>3</v>
       </c>
       <c r="G22" t="n">
-        <v>0.009777741920354702</v>
+        <v>0.01209398928722977</v>
       </c>
       <c r="H22" t="n">
         <v>1</v>

</xml_diff>